<commit_message>
se argego los cambios
</commit_message>
<xml_diff>
--- a/public/servicios_mas_pro.xlsx
+++ b/public/servicios_mas_pro.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\micar\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA2B16A-0FFA-4680-BD41-C4DB9F4B273A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -509,7 +510,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -581,12 +582,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -598,12 +599,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,20 +883,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,7 +924,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>100094</v>
       </c>
@@ -954,7 +953,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>100091</v>
       </c>
@@ -983,7 +982,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>8</v>
@@ -1010,7 +1009,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>100092</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>100112</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>100093</v>
       </c>
@@ -1097,7 +1096,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>100095</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>100101</v>
       </c>
@@ -1155,7 +1154,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>100099</v>
       </c>
@@ -1184,7 +1183,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>100100</v>
       </c>
@@ -1213,7 +1212,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>100100</v>
       </c>
@@ -1242,7 +1241,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>100110</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>18</v>
@@ -1298,7 +1297,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6" t="s">
         <v>19</v>
@@ -1325,7 +1324,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>100117</v>
       </c>
@@ -1354,7 +1353,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6" t="s">
         <v>21</v>
@@ -1381,7 +1380,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>22</v>
@@ -1408,7 +1407,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>100197</v>
       </c>
@@ -1437,7 +1436,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
         <v>24</v>
@@ -1464,7 +1463,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
         <v>25</v>
@@ -1491,7 +1490,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>100096</v>
       </c>
@@ -1520,7 +1519,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>100097</v>
       </c>
@@ -1549,7 +1548,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>100179</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>100098</v>
       </c>
@@ -1607,7 +1606,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>100133</v>
       </c>
@@ -1636,7 +1635,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>100134</v>
       </c>
@@ -1665,7 +1664,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>100105</v>
       </c>
@@ -1687,14 +1686,14 @@
       <c r="G28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="6">
         <v>45</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>100106</v>
       </c>
@@ -1716,14 +1715,14 @@
       <c r="G29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="6">
         <v>45</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>100104</v>
       </c>
@@ -1745,14 +1744,14 @@
       <c r="G30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="6">
         <v>45</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>100172</v>
       </c>
@@ -1774,14 +1773,14 @@
       <c r="G31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="6">
         <v>45</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>100135</v>
       </c>
@@ -1803,14 +1802,14 @@
       <c r="G32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="6">
         <v>45</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>100142</v>
       </c>
@@ -1832,14 +1831,14 @@
       <c r="G33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="6">
         <v>45</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>100138</v>
       </c>
@@ -1861,14 +1860,14 @@
       <c r="G34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="6">
         <v>45</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>100141</v>
       </c>
@@ -1890,14 +1889,14 @@
       <c r="G35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="6">
         <v>45</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>100152</v>
       </c>
@@ -1919,14 +1918,14 @@
       <c r="G36" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="6">
         <v>45</v>
       </c>
       <c r="I36" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>100139</v>
       </c>
@@ -1948,14 +1947,14 @@
       <c r="G37" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="6">
         <v>45</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>100151</v>
       </c>
@@ -1977,14 +1976,14 @@
       <c r="G38" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="6">
         <v>45</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>100143</v>
       </c>
@@ -2006,14 +2005,14 @@
       <c r="G39" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="6">
         <v>40</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>100140</v>
       </c>
@@ -2035,14 +2034,14 @@
       <c r="G40" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="6">
         <v>40</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>100120</v>
       </c>
@@ -2064,14 +2063,14 @@
       <c r="G41" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="6">
         <v>40</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>100119</v>
       </c>
@@ -2100,7 +2099,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>100123</v>
       </c>
@@ -2129,7 +2128,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>100126</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>100161</v>
       </c>
@@ -2187,7 +2186,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>100163</v>
       </c>
@@ -2216,7 +2215,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>100164</v>
       </c>
@@ -2245,7 +2244,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>100165</v>
       </c>
@@ -2274,7 +2273,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>100176</v>
       </c>
@@ -2296,14 +2295,14 @@
       <c r="G49" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H49" s="6">
         <v>45</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>100177</v>
       </c>
@@ -2325,14 +2324,14 @@
       <c r="G50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H50" s="9">
+      <c r="H50" s="6">
         <v>45</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>100178</v>
       </c>
@@ -2354,14 +2353,14 @@
       <c r="G51" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H51" s="6">
         <v>45</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>100192</v>
       </c>
@@ -2383,14 +2382,14 @@
       <c r="G52" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H52" s="9">
+      <c r="H52" s="6">
         <v>45</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>100193</v>
       </c>
@@ -2412,14 +2411,14 @@
       <c r="G53" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H53" s="9">
+      <c r="H53" s="6">
         <v>35</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>100198</v>
       </c>
@@ -2441,14 +2440,14 @@
       <c r="G54" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H54" s="6">
         <v>45</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>100199</v>
       </c>
@@ -2470,14 +2469,14 @@
       <c r="G55" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H55" s="9">
+      <c r="H55" s="6">
         <v>10</v>
       </c>
       <c r="I55" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>100201</v>
       </c>
@@ -2506,7 +2505,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
         <v>63</v>
       </c>
@@ -2523,7 +2522,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
         <v>64</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
         <v>65</v>
       </c>
@@ -2557,7 +2556,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
         <v>66</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>67</v>
       </c>
@@ -2591,7 +2590,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>68</v>
       </c>
@@ -2608,7 +2607,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>69</v>
       </c>
@@ -2625,7 +2624,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>70</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
         <v>71</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>72</v>
       </c>
@@ -2676,7 +2675,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
         <v>73</v>
       </c>
@@ -2693,7 +2692,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
         <v>74</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
         <v>75</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="70" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
         <v>76</v>
       </c>
@@ -2744,7 +2743,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>77</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="72" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
         <v>78</v>
       </c>
@@ -2778,7 +2777,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
         <v>79</v>
       </c>
@@ -2795,7 +2794,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="74" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
         <v>80</v>
       </c>
@@ -2812,7 +2811,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="75" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
         <v>81</v>
       </c>
@@ -2829,7 +2828,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
         <v>82</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
         <v>83</v>
       </c>
@@ -2863,7 +2862,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
         <v>84</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="4" t="s">
         <v>85</v>
       </c>
@@ -2897,7 +2896,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
         <v>86</v>
       </c>
@@ -2914,7 +2913,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="s">
         <v>87</v>
       </c>
@@ -2931,7 +2930,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="s">
         <v>88</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>89</v>
       </c>
@@ -2965,7 +2964,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="84" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
         <v>90</v>
       </c>
@@ -2982,7 +2981,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="s">
         <v>91</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="4" t="s">
         <v>92</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="4" t="s">
         <v>93</v>
       </c>
@@ -3033,7 +3032,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
         <v>94</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
         <v>95</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="90" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="4" t="s">
         <v>96</v>
       </c>
@@ -3084,7 +3083,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="91" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="4" t="s">
         <v>97</v>
       </c>
@@ -3101,7 +3100,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
         <v>98</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="93" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>99</v>
       </c>
@@ -3135,7 +3134,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>100</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="95" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
         <v>101</v>
       </c>
@@ -3169,7 +3168,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="s">
         <v>102</v>
       </c>
@@ -3186,7 +3185,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>103</v>
       </c>
@@ -3203,7 +3202,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="4" t="s">
         <v>104</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="s">
         <v>105</v>
       </c>
@@ -3237,7 +3236,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
         <v>106</v>
       </c>
@@ -3254,7 +3253,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" s="4" t="s">
         <v>107</v>
       </c>
@@ -3271,7 +3270,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" s="4" t="s">
         <v>108</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="4" t="s">
         <v>109</v>
       </c>
@@ -3305,7 +3304,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
         <v>110</v>
       </c>
@@ -3322,7 +3321,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="4" t="s">
         <v>111</v>
       </c>
@@ -3339,7 +3338,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="106" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="4" t="s">
         <v>112</v>
       </c>
@@ -3356,7 +3355,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="s">
         <v>113</v>
       </c>
@@ -3373,7 +3372,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="108" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="s">
         <v>114</v>
       </c>
@@ -3390,7 +3389,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="109" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" s="4" t="s">
         <v>115</v>
       </c>
@@ -3407,7 +3406,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="110" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="s">
         <v>116</v>
       </c>
@@ -3424,7 +3423,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="111" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" s="4" t="s">
         <v>117</v>
       </c>
@@ -3441,7 +3440,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="112" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="4" t="s">
         <v>118</v>
       </c>
@@ -3458,7 +3457,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="113" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" s="4" t="s">
         <v>119</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="114" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" s="4" t="s">
         <v>120</v>
       </c>
@@ -3492,7 +3491,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="115" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" s="4" t="s">
         <v>121</v>
       </c>
@@ -3509,7 +3508,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="116" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="4" t="s">
         <v>122</v>
       </c>
@@ -3526,7 +3525,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="117" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" s="4" t="s">
         <v>123</v>
       </c>
@@ -3543,7 +3542,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="118" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="4" t="s">
         <v>124</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="119" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="4" t="s">
         <v>125</v>
       </c>
@@ -3577,7 +3576,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="120" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" s="4" t="s">
         <v>126</v>
       </c>
@@ -3594,7 +3593,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="121" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" s="4" t="s">
         <v>127</v>
       </c>
@@ -3611,7 +3610,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="122" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" s="4" t="s">
         <v>128</v>
       </c>
@@ -3628,7 +3627,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="123" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
         <v>129</v>
       </c>
@@ -3645,7 +3644,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="124" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124" s="4" t="s">
         <v>130</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="125" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B125" s="4" t="s">
         <v>131</v>
       </c>
@@ -3679,7 +3678,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="126" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B126" s="4" t="s">
         <v>132</v>
       </c>
@@ -3696,7 +3695,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="127" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127" s="4" t="s">
         <v>133</v>
       </c>
@@ -3713,7 +3712,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="128" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B128" s="4" t="s">
         <v>134</v>
       </c>
@@ -3730,7 +3729,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="129" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="4" t="s">
         <v>135</v>
       </c>
@@ -3747,7 +3746,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="130" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
         <v>136</v>
       </c>
@@ -3764,7 +3763,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="131" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131" s="4" t="s">
         <v>137</v>
       </c>
@@ -3781,7 +3780,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="132" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132" s="4" t="s">
         <v>138</v>
       </c>
@@ -3798,7 +3797,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="133" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B133" s="4" t="s">
         <v>139</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="134" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134" s="4" t="s">
         <v>140</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="135" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="4" t="s">
         <v>141</v>
       </c>
@@ -3849,7 +3848,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="136" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="4" t="s">
         <v>142</v>
       </c>
@@ -3866,7 +3865,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="137" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="4" t="s">
         <v>143</v>
       </c>
@@ -3883,7 +3882,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="138" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
         <v>144</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="139" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" s="4" t="s">
         <v>145</v>
       </c>
@@ -3917,7 +3916,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="140" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" s="4" t="s">
         <v>146</v>
       </c>
@@ -3934,7 +3933,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="141" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" s="4" t="s">
         <v>147</v>
       </c>
@@ -3951,7 +3950,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="142" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="4" t="s">
         <v>148</v>
       </c>
@@ -3968,7 +3967,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="143" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" s="4" t="s">
         <v>149</v>
       </c>
@@ -3985,7 +3984,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="144" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" s="4" t="s">
         <v>150</v>
       </c>
@@ -4002,7 +4001,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="145" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B145" s="4" t="s">
         <v>151</v>
       </c>
@@ -4019,7 +4018,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="2:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
         <v>152</v>
       </c>
@@ -4037,13 +4036,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G146">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="servicio"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G146" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agrego los cambos
</commit_message>
<xml_diff>
--- a/public/servicios_mas_pro.xlsx
+++ b/public/servicios_mas_pro.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\micar\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA2B16A-0FFA-4680-BD41-C4DB9F4B273A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3576A8-1A2C-45A7-8D03-D39965A430B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$G$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$G$213</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="226">
   <si>
     <t>Código</t>
   </si>
@@ -384,36 +384,6 @@
     <t>TARJETA ENTEL (10)</t>
   </si>
   <si>
-    <t>TARJETA ENTEL (30)</t>
-  </si>
-  <si>
-    <t>TARJETA ENTEL (50)</t>
-  </si>
-  <si>
-    <t>TARJETA ENTEL (15)</t>
-  </si>
-  <si>
-    <t>TARJETA TIGO (20)</t>
-  </si>
-  <si>
-    <t>TARJETA TIGO (10)</t>
-  </si>
-  <si>
-    <t>TARJETA TIGO (30)</t>
-  </si>
-  <si>
-    <t>TARJETA TIGO (50)</t>
-  </si>
-  <si>
-    <t>TARJETA VIVA (10)</t>
-  </si>
-  <si>
-    <t>TARJETA VIVA (20)</t>
-  </si>
-  <si>
-    <t>TARJETA VIVA (30)</t>
-  </si>
-  <si>
     <t>SUPER BLUE</t>
   </si>
   <si>
@@ -480,9 +450,6 @@
     <t>SILICONA OPTIMUS</t>
   </si>
   <si>
-    <t>PORTA CELULAR</t>
-  </si>
-  <si>
     <t>CARGADOR DE CELULAR</t>
   </si>
   <si>
@@ -505,6 +472,240 @@
   </si>
   <si>
     <t>porcentaje</t>
+  </si>
+  <si>
+    <t>AIR FRESHENER</t>
+  </si>
+  <si>
+    <t>ESPONJA ARMORALL</t>
+  </si>
+  <si>
+    <t>ESPALDAR DE ASIENTOS</t>
+  </si>
+  <si>
+    <t>REFRESH YOUR FLOR-CHINELA (BAHAMAS)</t>
+  </si>
+  <si>
+    <t>REFRESH SPRAY PERFUMADO</t>
+  </si>
+  <si>
+    <t>SILICONA ARMOR SPRAY</t>
+  </si>
+  <si>
+    <t>LUCES DE TAXI</t>
+  </si>
+  <si>
+    <t>CERA AUTOMOTIVA MAXIRUBBER</t>
+  </si>
+  <si>
+    <t>SILICONE TEAM</t>
+  </si>
+  <si>
+    <t>CERA PULIDORA TURTLE WAX</t>
+  </si>
+  <si>
+    <t>SILICONA CERRAQUIMICA</t>
+  </si>
+  <si>
+    <t>TRAPO PARA LAVAR</t>
+  </si>
+  <si>
+    <t>SILICONA KIT</t>
+  </si>
+  <si>
+    <t>CERA KIT</t>
+  </si>
+  <si>
+    <t>NESCAFE SACHET</t>
+  </si>
+  <si>
+    <t>CERVEZA PACEÑA PALITO</t>
+  </si>
+  <si>
+    <t>SODA LATA</t>
+  </si>
+  <si>
+    <t>HELADO DE 1/2 LITRO</t>
+  </si>
+  <si>
+    <t>HELADO DUETO</t>
+  </si>
+  <si>
+    <t>GALLETA REX</t>
+  </si>
+  <si>
+    <t>HELADOS MILENIUM</t>
+  </si>
+  <si>
+    <t>HELADOS SALTINBANKI</t>
+  </si>
+  <si>
+    <t>HELADO CHOCO CHOCO</t>
+  </si>
+  <si>
+    <t>CICLON</t>
+  </si>
+  <si>
+    <t>BLACK</t>
+  </si>
+  <si>
+    <t>PROTECTAN</t>
+  </si>
+  <si>
+    <t>SILICONA PARA CUERO</t>
+  </si>
+  <si>
+    <t>CERA LUBRISTONE</t>
+  </si>
+  <si>
+    <t>PORTA CELULAR 360°</t>
+  </si>
+  <si>
+    <t>FRANELA CUERO</t>
+  </si>
+  <si>
+    <t>CENTRALSUL AROMA</t>
+  </si>
+  <si>
+    <t>PORTA CELULAR SAFARI</t>
+  </si>
+  <si>
+    <t>PORTA CELULAR FLY</t>
+  </si>
+  <si>
+    <t>AKRON LIMPIAPARABRISAS</t>
+  </si>
+  <si>
+    <t>PLATINIUM COLGAR</t>
+  </si>
+  <si>
+    <t>AQUARIUS 300 ML</t>
+  </si>
+  <si>
+    <t>SODA 300 ML</t>
+  </si>
+  <si>
+    <t>AQUARIUS 500 ML</t>
+  </si>
+  <si>
+    <t>SODA 500 ML</t>
+  </si>
+  <si>
+    <t>POWER 500 ML</t>
+  </si>
+  <si>
+    <t>POWER 1 LT</t>
+  </si>
+  <si>
+    <t>REFRESCO FRUTAS</t>
+  </si>
+  <si>
+    <t>MALTA - MALTIN</t>
+  </si>
+  <si>
+    <t>AGUA VITAL 500 ML</t>
+  </si>
+  <si>
+    <t>AGUA VITAL 2 LT</t>
+  </si>
+  <si>
+    <t>AGUA VITAL 3 LT</t>
+  </si>
+  <si>
+    <t>JUGO DEL VALLE 3 LT</t>
+  </si>
+  <si>
+    <t>SANTE</t>
+  </si>
+  <si>
+    <t>BELDENT</t>
+  </si>
+  <si>
+    <t>CLORETS</t>
+  </si>
+  <si>
+    <t>CIGARRO CAMEL DOBLE ACTIVA</t>
+  </si>
+  <si>
+    <t>ENCENDEDOR</t>
+  </si>
+  <si>
+    <t>CHICLE BUBALOO</t>
+  </si>
+  <si>
+    <t>NUCITA</t>
+  </si>
+  <si>
+    <t>GOMUCHO</t>
+  </si>
+  <si>
+    <t>MOMENTO</t>
+  </si>
+  <si>
+    <t>BATON</t>
+  </si>
+  <si>
+    <t>CHUPETES</t>
+  </si>
+  <si>
+    <t>GROSSO</t>
+  </si>
+  <si>
+    <t>BON O BON</t>
+  </si>
+  <si>
+    <t>PAÑUELO DESCECHABLE</t>
+  </si>
+  <si>
+    <t>CHUBI</t>
+  </si>
+  <si>
+    <t>NIKOLO</t>
+  </si>
+  <si>
+    <t>GALLETA WAFER GRANDE</t>
+  </si>
+  <si>
+    <t>GALLETA FRAC</t>
+  </si>
+  <si>
+    <t>GALLETA CHOCO SODA</t>
+  </si>
+  <si>
+    <t>GALLETA CLUB SOCIAL</t>
+  </si>
+  <si>
+    <t>GALLETA OREO</t>
+  </si>
+  <si>
+    <t>GALLETA RITZ QUESO</t>
+  </si>
+  <si>
+    <t>GOLAZO</t>
+  </si>
+  <si>
+    <t>CHIPILO</t>
+  </si>
+  <si>
+    <t>NACHOS - PAPA FRITAS</t>
+  </si>
+  <si>
+    <t>HELADOS VASITOS</t>
+  </si>
+  <si>
+    <t>HELADO BON O BON</t>
+  </si>
+  <si>
+    <t>HELADOS FRUTADOS</t>
+  </si>
+  <si>
+    <t>HELADOS CREMOSOS</t>
+  </si>
+  <si>
+    <t>CAFFE CLUB</t>
+  </si>
+  <si>
+    <t>SODA DE 2 LT</t>
   </si>
 </sst>
 </file>
@@ -582,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,6 +805,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,18 +1086,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I146"/>
+  <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B146"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,19 +1114,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>100094</v>
       </c>
@@ -950,10 +1152,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>100091</v>
       </c>
@@ -979,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>8</v>
@@ -1006,10 +1208,10 @@
         <v>0</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>100092</v>
       </c>
@@ -1035,10 +1237,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>100112</v>
       </c>
@@ -1064,10 +1266,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>100093</v>
       </c>
@@ -1093,10 +1295,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>100095</v>
       </c>
@@ -1122,10 +1324,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>100101</v>
       </c>
@@ -1151,10 +1353,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>100099</v>
       </c>
@@ -1180,10 +1382,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>100100</v>
       </c>
@@ -1209,10 +1411,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>100100</v>
       </c>
@@ -1238,10 +1440,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>100110</v>
       </c>
@@ -1267,10 +1469,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>18</v>
@@ -1294,10 +1496,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6" t="s">
         <v>19</v>
@@ -1321,10 +1523,10 @@
         <v>0</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>100117</v>
       </c>
@@ -1350,10 +1552,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6" t="s">
         <v>21</v>
@@ -1377,10 +1579,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>22</v>
@@ -1404,10 +1606,10 @@
         <v>0</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>100197</v>
       </c>
@@ -1433,10 +1635,10 @@
         <v>0</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
         <v>24</v>
@@ -1460,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
         <v>25</v>
@@ -1487,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>100096</v>
       </c>
@@ -1516,10 +1718,10 @@
         <v>10</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>100097</v>
       </c>
@@ -1545,10 +1747,10 @@
         <v>35</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>100179</v>
       </c>
@@ -1574,10 +1776,10 @@
         <v>10</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>100098</v>
       </c>
@@ -1603,10 +1805,10 @@
         <v>5</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>100133</v>
       </c>
@@ -1632,10 +1834,10 @@
         <v>40</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>100134</v>
       </c>
@@ -1661,10 +1863,10 @@
         <v>40</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>100105</v>
       </c>
@@ -1690,10 +1892,10 @@
         <v>45</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>100106</v>
       </c>
@@ -1719,10 +1921,10 @@
         <v>45</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>100104</v>
       </c>
@@ -1748,10 +1950,10 @@
         <v>45</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>100172</v>
       </c>
@@ -1777,10 +1979,10 @@
         <v>45</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>100135</v>
       </c>
@@ -1806,10 +2008,10 @@
         <v>45</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>100142</v>
       </c>
@@ -1835,10 +2037,10 @@
         <v>45</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>100138</v>
       </c>
@@ -1864,10 +2066,10 @@
         <v>45</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>100141</v>
       </c>
@@ -1893,10 +2095,10 @@
         <v>45</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>100152</v>
       </c>
@@ -1922,10 +2124,10 @@
         <v>45</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>100139</v>
       </c>
@@ -1951,10 +2153,10 @@
         <v>45</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>100151</v>
       </c>
@@ -1980,10 +2182,10 @@
         <v>45</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>100143</v>
       </c>
@@ -2009,10 +2211,10 @@
         <v>40</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>100140</v>
       </c>
@@ -2038,10 +2240,10 @@
         <v>40</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>100120</v>
       </c>
@@ -2067,10 +2269,10 @@
         <v>40</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>100119</v>
       </c>
@@ -2096,10 +2298,10 @@
         <v>0</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>100123</v>
       </c>
@@ -2125,10 +2327,10 @@
         <v>0</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>100126</v>
       </c>
@@ -2154,10 +2356,10 @@
         <v>45</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>100161</v>
       </c>
@@ -2183,10 +2385,10 @@
         <v>0</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>100163</v>
       </c>
@@ -2212,10 +2414,10 @@
         <v>0</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>100164</v>
       </c>
@@ -2241,10 +2443,10 @@
         <v>0</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>100165</v>
       </c>
@@ -2270,10 +2472,10 @@
         <v>0</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>100176</v>
       </c>
@@ -2299,10 +2501,10 @@
         <v>45</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>100177</v>
       </c>
@@ -2328,10 +2530,10 @@
         <v>45</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>100178</v>
       </c>
@@ -2357,10 +2559,10 @@
         <v>45</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>100192</v>
       </c>
@@ -2386,10 +2588,10 @@
         <v>45</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>100193</v>
       </c>
@@ -2415,10 +2617,10 @@
         <v>35</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>100198</v>
       </c>
@@ -2444,10 +2646,10 @@
         <v>45</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>100199</v>
       </c>
@@ -2473,10 +2675,10 @@
         <v>10</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>100201</v>
       </c>
@@ -2502,10 +2704,10 @@
         <v>45</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B57" s="4" t="s">
         <v>63</v>
       </c>
@@ -2519,10 +2721,10 @@
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B58" s="4" t="s">
         <v>64</v>
       </c>
@@ -2533,185 +2735,185 @@
         <v>20</v>
       </c>
       <c r="F58" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="5">
+        <v>20</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B60" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="5">
+        <v>25</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B61" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" s="5">
+      <c r="D61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="5">
         <v>30</v>
       </c>
-      <c r="F59" s="4">
-        <v>0</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+      <c r="F61" s="4">
+        <v>15</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B62" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" s="5">
+      <c r="D62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="5">
         <v>20</v>
       </c>
-      <c r="F60" s="4">
-        <v>1</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+      <c r="F62" s="4">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B63" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="5">
+      <c r="D63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="5">
         <v>40</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F63" s="4">
         <v>17</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+      <c r="G63" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B64" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="5">
+      <c r="D64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="5">
         <v>5</v>
       </c>
-      <c r="F62" s="4">
-        <v>35</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+      <c r="F64" s="4">
+        <v>16</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="5">
+      <c r="D65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="5">
         <v>7</v>
       </c>
-      <c r="F63" s="4">
-        <v>263</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+      <c r="F65" s="4">
+        <v>198</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B66" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="5">
+        <v>25</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B67" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="5">
+      <c r="D67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="5">
         <v>60</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F67" s="4">
         <v>3</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+      <c r="G67" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B68" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" s="5">
+      <c r="D68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="5">
         <v>60</v>
       </c>
-      <c r="F65" s="4">
+      <c r="F68" s="4">
         <v>2</v>
       </c>
-      <c r="G65" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+      <c r="G68" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" s="5">
-        <v>20</v>
-      </c>
-      <c r="F66" s="4">
-        <v>11</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" s="5">
-        <v>30</v>
-      </c>
-      <c r="F67" s="4">
-        <v>4</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68" s="5">
-        <v>10</v>
-      </c>
-      <c r="F68" s="4">
-        <v>6</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>6</v>
@@ -2720,83 +2922,83 @@
         <v>20</v>
       </c>
       <c r="F69" s="4">
+        <v>11</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B70" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="5">
+        <v>30</v>
+      </c>
+      <c r="F70" s="4">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" s="5">
+        <v>10</v>
+      </c>
+      <c r="F71" s="4">
         <v>3</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+      <c r="G71" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B72" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="5">
+        <v>20</v>
+      </c>
+      <c r="F72" s="4">
+        <v>3</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B73" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E70" s="5">
+      <c r="D73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="5">
         <v>50</v>
       </c>
-      <c r="F70" s="4">
-        <v>18</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+      <c r="F73" s="4">
+        <v>22</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B74" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E71" s="5">
-        <v>35</v>
-      </c>
-      <c r="F71" s="4">
-        <v>2</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" s="5">
-        <v>25</v>
-      </c>
-      <c r="F72" s="4">
-        <v>16</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="5">
-        <v>40</v>
-      </c>
-      <c r="F73" s="4">
-        <v>4</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
@@ -2805,49 +3007,49 @@
         <v>35</v>
       </c>
       <c r="F74" s="4">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E75" s="5">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F75" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E76" s="5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F76" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>6</v>
@@ -2856,49 +3058,49 @@
         <v>35</v>
       </c>
       <c r="F77" s="4">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E78" s="5">
+        <v>35</v>
+      </c>
+      <c r="F78" s="4">
+        <v>2</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B79" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="5">
         <v>30</v>
       </c>
-      <c r="F78" s="4">
-        <v>6</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" s="5">
-        <v>50</v>
-      </c>
       <c r="F79" s="4">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B80" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>6</v>
@@ -2907,202 +3109,202 @@
         <v>35</v>
       </c>
       <c r="F80" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="5">
+        <v>30</v>
+      </c>
+      <c r="F81" s="4">
+        <v>2</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B82" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" s="5">
+        <v>20</v>
+      </c>
+      <c r="F82" s="4">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B83" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="5">
+        <v>50</v>
+      </c>
+      <c r="F83" s="4">
+        <v>10</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B84" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="5">
+        <v>35</v>
+      </c>
+      <c r="F84" s="4">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B85" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="5">
+        <v>20</v>
+      </c>
+      <c r="F85" s="4">
+        <v>0</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B86" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E81" s="5">
+      <c r="D86" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="5">
         <v>35</v>
       </c>
-      <c r="F81" s="4">
-        <v>76</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+      <c r="F86" s="4">
+        <v>105</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B87" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E82" s="5">
+      <c r="D87" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="5">
         <v>40</v>
       </c>
-      <c r="F82" s="4">
-        <v>6</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+      <c r="F87" s="4">
+        <v>2</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B88" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E83" s="5">
+      <c r="D88" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" s="5">
         <v>25</v>
       </c>
-      <c r="F83" s="4">
-        <v>2</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+      <c r="F88" s="4">
+        <v>0</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B89" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E84" s="5">
+      <c r="D89" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" s="5">
         <v>30</v>
       </c>
-      <c r="F84" s="4">
-        <v>1</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+      <c r="F89" s="4">
+        <v>0</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B90" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E85" s="5">
+      <c r="D90" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" s="5">
         <v>35</v>
       </c>
-      <c r="F85" s="4">
-        <v>17</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+      <c r="F90" s="4">
+        <v>29</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B91" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E86" s="5">
+      <c r="D91" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="5">
         <v>30</v>
       </c>
-      <c r="F86" s="4">
-        <v>4</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+      <c r="F91" s="4">
+        <v>0</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B92" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E87" s="5">
-        <v>35</v>
-      </c>
-      <c r="F87" s="4">
-        <v>11</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E88" s="5">
-        <v>40</v>
-      </c>
-      <c r="F88" s="4">
-        <v>8</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E89" s="5">
-        <v>35</v>
-      </c>
-      <c r="F89" s="4">
-        <v>8</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E90" s="5">
-        <v>100</v>
-      </c>
-      <c r="F90" s="4">
-        <v>1</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E91" s="5">
-        <v>35</v>
-      </c>
-      <c r="F91" s="4">
-        <v>1</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>6</v>
@@ -3111,627 +3313,627 @@
         <v>35</v>
       </c>
       <c r="F92" s="4">
+        <v>9</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B93" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="5">
+        <v>40</v>
+      </c>
+      <c r="F93" s="4">
+        <v>8</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B94" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" s="5">
+        <v>35</v>
+      </c>
+      <c r="F94" s="4">
+        <v>3</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B95" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="5">
+        <v>100</v>
+      </c>
+      <c r="F95" s="4">
         <v>1</v>
       </c>
-      <c r="G92" s="3" t="s">
+      <c r="G95" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B96" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" s="5">
+        <v>35</v>
+      </c>
+      <c r="F96" s="4">
+        <v>0</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B97" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" s="5">
-        <v>60</v>
-      </c>
-      <c r="F93" s="4">
-        <v>4</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E94" s="5">
-        <v>30</v>
-      </c>
-      <c r="F94" s="4">
-        <v>2</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E95" s="5">
+      <c r="D97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" s="5">
+        <v>25</v>
+      </c>
+      <c r="F97" s="4">
+        <v>0</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B98" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" s="5">
         <v>35</v>
-      </c>
-      <c r="F95" s="4">
-        <v>4</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E96" s="5">
-        <v>40</v>
-      </c>
-      <c r="F96" s="4">
-        <v>24</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E97" s="5">
-        <v>15</v>
-      </c>
-      <c r="F97" s="4">
-        <v>15</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98" s="5">
-        <v>10</v>
       </c>
       <c r="F98" s="4">
         <v>5</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B99" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="5">
+        <v>60</v>
+      </c>
+      <c r="F99" s="4">
+        <v>4</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B100" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="5">
+        <v>20</v>
+      </c>
+      <c r="F100" s="4">
+        <v>0</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B101" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="5">
+        <v>30</v>
+      </c>
+      <c r="F101" s="4">
+        <v>3</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B102" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102" s="5">
+        <v>30</v>
+      </c>
+      <c r="F102" s="4">
+        <v>0</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B103" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="5">
+        <v>35</v>
+      </c>
+      <c r="F103" s="4">
+        <v>2</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B104" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="5">
+        <v>30</v>
+      </c>
+      <c r="F104" s="4">
+        <v>0</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B105" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="5">
+        <v>40</v>
+      </c>
+      <c r="F105" s="4">
+        <v>24</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B106" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" s="5">
+        <v>35</v>
+      </c>
+      <c r="F106" s="4">
+        <v>0</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B107" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" s="5">
+        <v>15</v>
+      </c>
+      <c r="F107" s="4">
+        <v>14</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B108" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" s="5">
+        <v>10</v>
+      </c>
+      <c r="F108" s="4">
+        <v>4</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B109" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E99" s="5">
+      <c r="D109" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="5">
         <v>5</v>
       </c>
-      <c r="F99" s="4">
-        <v>9</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+      <c r="F109" s="4">
+        <v>8</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B110" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" s="5">
+      <c r="D110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" s="5">
         <v>100</v>
       </c>
-      <c r="F100" s="4">
+      <c r="F110" s="4">
         <v>5</v>
       </c>
-      <c r="G100" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+      <c r="G110" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B111" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="5">
+      <c r="D111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" s="5">
         <v>2.5</v>
       </c>
-      <c r="F101" s="4">
+      <c r="F111" s="4">
+        <v>28</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B112" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" s="5">
+        <v>3</v>
+      </c>
+      <c r="F112" s="4">
+        <v>141</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B113" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="5">
+        <v>180</v>
+      </c>
+      <c r="F113" s="4">
+        <v>0</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B114" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" s="5">
+        <v>20</v>
+      </c>
+      <c r="F114" s="4">
+        <v>10</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B115" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="5">
+        <v>10</v>
+      </c>
+      <c r="F115" s="4">
+        <v>1</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B116" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" s="5">
+        <v>30</v>
+      </c>
+      <c r="F116" s="4">
+        <v>1</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B117" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" s="5">
+        <v>20</v>
+      </c>
+      <c r="F117" s="4">
+        <v>0</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B118" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" s="5">
+        <v>10</v>
+      </c>
+      <c r="F118" s="4">
+        <v>12</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B119" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" s="5">
+        <v>15</v>
+      </c>
+      <c r="F119" s="4">
+        <v>3</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B120" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E120" s="5">
+        <v>10</v>
+      </c>
+      <c r="F120" s="4">
+        <v>0</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B121" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" s="5">
+        <v>10</v>
+      </c>
+      <c r="F121" s="4">
+        <v>0</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B122" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122" s="5">
+        <v>5</v>
+      </c>
+      <c r="F122" s="4">
+        <v>2</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B123" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123" s="5">
+        <v>30</v>
+      </c>
+      <c r="F123" s="4">
+        <v>8</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B124" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" s="5">
+        <v>30</v>
+      </c>
+      <c r="F124" s="4">
+        <v>2</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B125" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" s="5">
+        <v>1</v>
+      </c>
+      <c r="F125" s="4">
+        <v>0</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B126" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E126" s="5">
         <v>11</v>
       </c>
-      <c r="G101" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" s="5">
-        <v>3</v>
-      </c>
-      <c r="F102" s="4">
-        <v>118</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E103" s="5">
-        <v>20</v>
-      </c>
-      <c r="F103" s="4">
-        <v>8</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E104" s="5">
+      <c r="F126" s="4">
+        <v>0</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B127" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" s="5">
+        <v>6</v>
+      </c>
+      <c r="F127" s="4">
         <v>10</v>
       </c>
-      <c r="F104" s="4">
+      <c r="G127" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B128" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E128" s="5">
         <v>5</v>
       </c>
-      <c r="G104" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E105" s="5">
-        <v>30</v>
-      </c>
-      <c r="F105" s="4">
-        <v>8</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E106" s="5">
-        <v>20</v>
-      </c>
-      <c r="F106" s="4">
-        <v>0</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E107" s="5">
-        <v>10</v>
-      </c>
-      <c r="F107" s="4">
-        <v>15</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E108" s="5">
-        <v>15</v>
-      </c>
-      <c r="F108" s="4">
-        <v>3</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="5">
-        <v>10</v>
-      </c>
-      <c r="F109" s="4">
-        <v>25</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E110" s="5">
-        <v>5</v>
-      </c>
-      <c r="F110" s="4">
-        <v>3</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E111" s="5">
-        <v>11</v>
-      </c>
-      <c r="F111" s="4">
-        <v>7</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E112" s="5">
-        <v>30</v>
-      </c>
-      <c r="F112" s="4">
-        <v>6</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E113" s="5">
-        <v>50</v>
-      </c>
-      <c r="F113" s="4">
-        <v>0</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E114" s="5">
-        <v>15</v>
-      </c>
-      <c r="F114" s="4">
-        <v>8</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E115" s="5">
-        <v>20</v>
-      </c>
-      <c r="F115" s="4">
-        <v>9</v>
-      </c>
-      <c r="G115" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E116" s="5">
-        <v>11</v>
-      </c>
-      <c r="F116" s="4">
-        <v>11</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E117" s="5">
-        <v>30</v>
-      </c>
-      <c r="F117" s="4">
-        <v>11</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B118" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E118" s="5">
-        <v>50</v>
-      </c>
-      <c r="F118" s="4">
-        <v>10</v>
-      </c>
-      <c r="G118" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E119" s="5">
-        <v>11</v>
-      </c>
-      <c r="F119" s="4">
-        <v>0</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E120" s="5">
-        <v>20</v>
-      </c>
-      <c r="F120" s="4">
-        <v>0</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E121" s="5">
-        <v>30</v>
-      </c>
-      <c r="F121" s="4">
-        <v>0</v>
-      </c>
-      <c r="G121" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E122" s="5">
-        <v>3.5</v>
-      </c>
-      <c r="F122" s="4">
-        <v>5</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E123" s="5">
-        <v>7</v>
-      </c>
-      <c r="F123" s="4">
-        <v>5</v>
-      </c>
-      <c r="G123" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E124" s="5">
-        <v>8</v>
-      </c>
-      <c r="F124" s="4">
-        <v>0</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E125" s="5">
-        <v>20</v>
-      </c>
-      <c r="F125" s="4">
-        <v>0</v>
-      </c>
-      <c r="G125" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E126" s="5">
-        <v>15</v>
-      </c>
-      <c r="F126" s="4">
-        <v>10</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E127" s="5">
-        <v>2</v>
-      </c>
-      <c r="F127" s="4">
-        <v>88</v>
-      </c>
-      <c r="G127" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E128" s="5">
-        <v>25</v>
-      </c>
       <c r="F128" s="4">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B129" s="4" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>6</v>
@@ -3740,253 +3942,253 @@
         <v>10</v>
       </c>
       <c r="F129" s="4">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B130" s="4" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E130" s="5">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="F130" s="4">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B131" s="4" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E131" s="5">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F131" s="4">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B132" s="4" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E132" s="5">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="F132" s="4">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B133" s="4" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E133" s="5">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F133" s="4">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B134" s="4" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E134" s="5">
-        <v>35</v>
+        <v>3.5</v>
       </c>
       <c r="F134" s="4">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B135" s="4" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E135" s="5">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="F135" s="4">
         <v>5</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B136" s="4" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E136" s="5">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F136" s="4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B137" s="4" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E137" s="5">
-        <v>35</v>
+        <v>3.5</v>
       </c>
       <c r="F137" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B138" s="4" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E138" s="5">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F138" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B139" s="4" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E139" s="5">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="F139" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B140" s="4" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E140" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F140" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B141" s="4" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E141" s="5">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="F141" s="4">
         <v>4</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B142" s="4" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E142" s="5">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="F142" s="4">
         <v>2</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B143" s="4" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E143" s="5">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F143" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B144" s="4" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>6</v>
@@ -3998,45 +4200,1184 @@
         <v>0</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B145" s="4" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E145" s="5">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F145" s="4">
         <v>3</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B146" s="4" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E146" s="5">
+        <v>75</v>
+      </c>
+      <c r="F146" s="4">
+        <v>0</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>127</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E147" s="9">
         <v>20</v>
       </c>
-      <c r="F146" s="4">
+      <c r="F147">
+        <v>14</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>128</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E148" s="9">
+        <v>60</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>129</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E149" s="9">
+        <v>20</v>
+      </c>
+      <c r="F149">
+        <v>8</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
+        <v>174</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E150" s="9">
+        <v>40</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>175</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E151" s="9">
+        <v>40</v>
+      </c>
+      <c r="F151">
+        <v>7</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
+        <v>130</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E152" s="9">
+        <v>35</v>
+      </c>
+      <c r="F152">
+        <v>2</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
+        <v>131</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E153" s="9">
+        <v>40</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B154" t="s">
+        <v>132</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E154" s="9">
+        <v>35</v>
+      </c>
+      <c r="F154">
+        <v>1</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
+        <v>133</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E155" s="9">
+        <v>35</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B156" t="s">
+        <v>134</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E156" s="9">
+        <v>100</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B157" t="s">
+        <v>135</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E157" s="9">
+        <v>30</v>
+      </c>
+      <c r="F157">
+        <v>2</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B158" t="s">
+        <v>136</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E158" s="9">
+        <v>30</v>
+      </c>
+      <c r="F158">
+        <v>22</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B159" t="s">
+        <v>137</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E159" s="9">
+        <v>85</v>
+      </c>
+      <c r="F159">
         <v>3</v>
       </c>
-      <c r="G146" s="3" t="s">
-        <v>153</v>
+      <c r="G159" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B160" t="s">
+        <v>138</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E160" s="9">
+        <v>80</v>
+      </c>
+      <c r="F160">
+        <v>2</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B161" t="s">
+        <v>139</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E161" s="9">
+        <v>20</v>
+      </c>
+      <c r="F161">
+        <v>4</v>
+      </c>
+      <c r="G161" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B162" t="s">
+        <v>176</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E162" s="9">
+        <v>40</v>
+      </c>
+      <c r="F162">
+        <v>1</v>
+      </c>
+      <c r="G162" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B163" t="s">
+        <v>140</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E163" s="9">
+        <v>40</v>
+      </c>
+      <c r="F163">
+        <v>2</v>
+      </c>
+      <c r="G163" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B164" t="s">
+        <v>141</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E164" s="9">
+        <v>20</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B165" t="s">
+        <v>177</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E165" s="9">
+        <v>20</v>
+      </c>
+      <c r="F165">
+        <v>2</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B166" t="s">
+        <v>178</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E166" s="9">
+        <v>15</v>
+      </c>
+      <c r="F166">
+        <v>11</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B167" t="s">
+        <v>179</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E167" s="9">
+        <v>50</v>
+      </c>
+      <c r="F167">
+        <v>2</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B168" t="s">
+        <v>180</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E168" s="9">
+        <v>30</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B169" t="s">
+        <v>181</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E169" s="9">
+        <v>35</v>
+      </c>
+      <c r="F169">
+        <v>5</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B170" t="s">
+        <v>182</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E170" s="9">
+        <v>10</v>
+      </c>
+      <c r="F170">
+        <v>22</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B171" t="s">
+        <v>183</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E171" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="F171">
+        <v>24</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B172" t="s">
+        <v>184</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E172" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="F172">
+        <v>48</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B173" t="s">
+        <v>185</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E173" s="9">
+        <v>6</v>
+      </c>
+      <c r="F173">
+        <v>16</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B174" t="s">
+        <v>186</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E174" s="9">
+        <v>6</v>
+      </c>
+      <c r="F174">
+        <v>47</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B175" t="s">
+        <v>187</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E175" s="9">
+        <v>7</v>
+      </c>
+      <c r="F175">
+        <v>15</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B176" t="s">
+        <v>188</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E176" s="9">
+        <v>10</v>
+      </c>
+      <c r="F176">
+        <v>18</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B177" t="s">
+        <v>189</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E177" s="9">
+        <v>3</v>
+      </c>
+      <c r="F177">
+        <v>6</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B178" t="s">
+        <v>190</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E178" s="9">
+        <v>5</v>
+      </c>
+      <c r="F178">
+        <v>25</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B179" t="s">
+        <v>191</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E179" s="9">
+        <v>5</v>
+      </c>
+      <c r="F179">
+        <v>5</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B180" t="s">
+        <v>192</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E180" s="9">
+        <v>7</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B181" t="s">
+        <v>193</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E181" s="9">
+        <v>9</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B182" t="s">
+        <v>194</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E182" s="9">
+        <v>16</v>
+      </c>
+      <c r="F182">
+        <v>4</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B183" t="s">
+        <v>195</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E183" s="9">
+        <v>7</v>
+      </c>
+      <c r="F183">
+        <v>54</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B184" t="s">
+        <v>196</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E184" s="9">
+        <v>3</v>
+      </c>
+      <c r="F184">
+        <v>10</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B185" t="s">
+        <v>197</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E185" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F185">
+        <v>22</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B186" t="s">
+        <v>198</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E186" s="9">
+        <v>1</v>
+      </c>
+      <c r="F186">
+        <v>217</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B187" t="s">
+        <v>199</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E187" s="9">
+        <v>1</v>
+      </c>
+      <c r="F187">
+        <v>38</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B188" t="s">
+        <v>200</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E188" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F188">
+        <v>33</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="189" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B189" t="s">
+        <v>201</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E189" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="190" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B190" t="s">
+        <v>202</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E190" s="9">
+        <v>1</v>
+      </c>
+      <c r="F190">
+        <v>7</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="191" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B191" t="s">
+        <v>203</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E191" s="9">
+        <v>3</v>
+      </c>
+      <c r="F191">
+        <v>9</v>
+      </c>
+      <c r="G191" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B192" t="s">
+        <v>204</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E192" s="9">
+        <v>2</v>
+      </c>
+      <c r="F192">
+        <v>10</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B193" t="s">
+        <v>205</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E193" s="9">
+        <v>1</v>
+      </c>
+      <c r="F193">
+        <v>29</v>
+      </c>
+      <c r="G193" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="194" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B194" t="s">
+        <v>206</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E194" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F194">
+        <v>39</v>
+      </c>
+      <c r="G194" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B195" t="s">
+        <v>207</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E195" s="9">
+        <v>1</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="196" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B196" t="s">
+        <v>208</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E196" s="9">
+        <v>2</v>
+      </c>
+      <c r="F196">
+        <v>6</v>
+      </c>
+      <c r="G196" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B197" t="s">
+        <v>209</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E197" s="9">
+        <v>2</v>
+      </c>
+      <c r="F197">
+        <v>13</v>
+      </c>
+      <c r="G197" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B198" t="s">
+        <v>210</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E198" s="9">
+        <v>3</v>
+      </c>
+      <c r="F198">
+        <v>19</v>
+      </c>
+      <c r="G198" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="199" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B199" t="s">
+        <v>211</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E199" s="9">
+        <v>4</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="G199" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="200" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B200" t="s">
+        <v>212</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E200" s="9">
+        <v>3</v>
+      </c>
+      <c r="F200">
+        <v>11</v>
+      </c>
+      <c r="G200" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="201" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B201" t="s">
+        <v>213</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E201" s="9">
+        <v>3</v>
+      </c>
+      <c r="F201">
+        <v>12</v>
+      </c>
+      <c r="G201" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="202" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B202" t="s">
+        <v>214</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E202" s="9">
+        <v>2</v>
+      </c>
+      <c r="F202">
+        <v>25</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="203" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B203" t="s">
+        <v>215</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E203" s="9">
+        <v>2</v>
+      </c>
+      <c r="F203">
+        <v>6</v>
+      </c>
+      <c r="G203" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="204" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B204" t="s">
+        <v>216</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E204" s="9">
+        <v>3</v>
+      </c>
+      <c r="F204">
+        <v>6</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="205" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B205" t="s">
+        <v>217</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E205" s="9">
+        <v>1</v>
+      </c>
+      <c r="F205">
+        <v>2</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="206" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B206" t="s">
+        <v>218</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E206" s="9">
+        <v>2</v>
+      </c>
+      <c r="F206">
+        <v>1</v>
+      </c>
+      <c r="G206" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="207" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B207" t="s">
+        <v>219</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E207" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="F207">
+        <v>15</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="208" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B208" t="s">
+        <v>220</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E208" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="F208">
+        <v>71</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="209" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B209" t="s">
+        <v>221</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E209" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="F209">
+        <v>42</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B210" t="s">
+        <v>222</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E210" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="F210">
+        <v>36</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="211" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B211" t="s">
+        <v>223</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E211" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="F211">
+        <v>20</v>
+      </c>
+      <c r="G211" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B212" t="s">
+        <v>224</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E212" s="9">
+        <v>7</v>
+      </c>
+      <c r="F212">
+        <v>49</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="213" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B213" t="s">
+        <v>225</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E213" s="9">
+        <v>12</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="G213" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G146" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G213" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agreog los utlimos cambios
</commit_message>
<xml_diff>
--- a/public/servicios_mas_pro.xlsx
+++ b/public/servicios_mas_pro.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\micar\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39CFEC1-E01A-463C-9DFA-0F28857E9FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -228,9 +227,6 @@
     <t>EXOTICA</t>
   </si>
   <si>
-    <t>REFIL EXOTICA</t>
-  </si>
-  <si>
     <t>ELEGANCE</t>
   </si>
   <si>
@@ -471,12 +467,6 @@
     <t>porcentaje</t>
   </si>
   <si>
-    <t>AIR FRESHENER</t>
-  </si>
-  <si>
-    <t>ESPONJA ARMORALL</t>
-  </si>
-  <si>
     <t>ESPALDAR DE ASIENTOS</t>
   </si>
   <si>
@@ -681,9 +671,6 @@
     <t>GOLAZO</t>
   </si>
   <si>
-    <t>CHIPILO</t>
-  </si>
-  <si>
     <t>NACHOS - PAPA FRITAS</t>
   </si>
   <si>
@@ -706,12 +693,24 @@
   </si>
   <si>
     <t>AGUA VITAL 1 LT</t>
+  </si>
+  <si>
+    <t>ALOE VERA</t>
+  </si>
+  <si>
+    <t>TURRON</t>
+  </si>
+  <si>
+    <t>FLAN</t>
+  </si>
+  <si>
+    <t>COFLER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1085,19 +1084,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="H195" sqref="H195"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1114,19 +1113,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>100094</v>
       </c>
@@ -1152,10 +1151,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>100091</v>
       </c>
@@ -1181,10 +1180,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>8</v>
@@ -1208,10 +1207,10 @@
         <v>0</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>100092</v>
       </c>
@@ -1237,10 +1236,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>100112</v>
       </c>
@@ -1266,10 +1265,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>100093</v>
       </c>
@@ -1295,10 +1294,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>100095</v>
       </c>
@@ -1324,10 +1323,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>100101</v>
       </c>
@@ -1353,10 +1352,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>100099</v>
       </c>
@@ -1382,10 +1381,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>100100</v>
       </c>
@@ -1411,10 +1410,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>100100</v>
       </c>
@@ -1440,10 +1439,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>100110</v>
       </c>
@@ -1469,10 +1468,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>18</v>
@@ -1496,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6" t="s">
         <v>19</v>
@@ -1523,10 +1522,10 @@
         <v>0</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>100117</v>
       </c>
@@ -1552,10 +1551,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6" t="s">
         <v>21</v>
@@ -1579,10 +1578,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>22</v>
@@ -1606,10 +1605,10 @@
         <v>0</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>100197</v>
       </c>
@@ -1635,10 +1634,10 @@
         <v>0</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
         <v>24</v>
@@ -1662,10 +1661,10 @@
         <v>0</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
         <v>25</v>
@@ -1689,10 +1688,10 @@
         <v>0</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>100096</v>
       </c>
@@ -1718,10 +1717,10 @@
         <v>10</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>100097</v>
       </c>
@@ -1747,10 +1746,10 @@
         <v>35</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>100179</v>
       </c>
@@ -1776,10 +1775,10 @@
         <v>10</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>100098</v>
       </c>
@@ -1805,10 +1804,10 @@
         <v>5</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>100133</v>
       </c>
@@ -1834,10 +1833,10 @@
         <v>40</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>100134</v>
       </c>
@@ -1863,10 +1862,10 @@
         <v>40</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>100105</v>
       </c>
@@ -1892,10 +1891,10 @@
         <v>45</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>100106</v>
       </c>
@@ -1921,10 +1920,10 @@
         <v>45</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>100104</v>
       </c>
@@ -1950,10 +1949,10 @@
         <v>45</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>100172</v>
       </c>
@@ -1979,10 +1978,10 @@
         <v>45</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>100135</v>
       </c>
@@ -2008,10 +2007,10 @@
         <v>45</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>100142</v>
       </c>
@@ -2037,10 +2036,10 @@
         <v>45</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>100138</v>
       </c>
@@ -2066,10 +2065,10 @@
         <v>45</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>100141</v>
       </c>
@@ -2095,10 +2094,10 @@
         <v>45</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>100152</v>
       </c>
@@ -2124,10 +2123,10 @@
         <v>45</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>100139</v>
       </c>
@@ -2153,10 +2152,10 @@
         <v>45</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>100151</v>
       </c>
@@ -2182,10 +2181,10 @@
         <v>45</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>100143</v>
       </c>
@@ -2211,10 +2210,10 @@
         <v>40</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>100140</v>
       </c>
@@ -2240,10 +2239,10 @@
         <v>40</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>100120</v>
       </c>
@@ -2269,10 +2268,10 @@
         <v>40</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>100119</v>
       </c>
@@ -2298,10 +2297,10 @@
         <v>0</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>100123</v>
       </c>
@@ -2327,10 +2326,10 @@
         <v>0</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>100126</v>
       </c>
@@ -2356,10 +2355,10 @@
         <v>45</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>100161</v>
       </c>
@@ -2385,10 +2384,10 @@
         <v>0</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>100163</v>
       </c>
@@ -2414,10 +2413,10 @@
         <v>0</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>100164</v>
       </c>
@@ -2443,10 +2442,10 @@
         <v>0</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>100165</v>
       </c>
@@ -2472,10 +2471,10 @@
         <v>0</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>100176</v>
       </c>
@@ -2501,10 +2500,10 @@
         <v>45</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>100177</v>
       </c>
@@ -2530,10 +2529,10 @@
         <v>45</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>100178</v>
       </c>
@@ -2559,10 +2558,10 @@
         <v>45</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>100192</v>
       </c>
@@ -2588,10 +2587,10 @@
         <v>45</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>100193</v>
       </c>
@@ -2617,10 +2616,10 @@
         <v>35</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>100198</v>
       </c>
@@ -2646,10 +2645,10 @@
         <v>45</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>100199</v>
       </c>
@@ -2675,10 +2674,10 @@
         <v>10</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>100201</v>
       </c>
@@ -2704,10 +2703,10 @@
         <v>45</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B57" s="4" t="s">
         <v>63</v>
       </c>
@@ -2721,10 +2720,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B58" s="4" t="s">
         <v>64</v>
       </c>
@@ -2738,44 +2737,44 @@
         <v>8</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" s="4" t="s">
-        <v>147</v>
+        <v>222</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F59" s="4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B60" s="4" t="s">
-        <v>148</v>
+        <v>223</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E60" s="5">
-        <v>25</v>
+        <v>1.5</v>
       </c>
       <c r="F60" s="4">
         <v>0</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B61" s="4" t="s">
         <v>65</v>
       </c>
@@ -2786,32 +2785,32 @@
         <v>30</v>
       </c>
       <c r="F61" s="4">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B62" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="5">
+        <v>3</v>
+      </c>
+      <c r="F62" s="4">
+        <v>5</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B63" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="5">
-        <v>20</v>
-      </c>
-      <c r="F62" s="4">
-        <v>0</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
@@ -2820,15 +2819,15 @@
         <v>40</v>
       </c>
       <c r="F63" s="4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B64" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
@@ -2837,15 +2836,15 @@
         <v>5</v>
       </c>
       <c r="F64" s="4">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>6</v>
@@ -2854,15 +2853,15 @@
         <v>7</v>
       </c>
       <c r="F65" s="4">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>6</v>
@@ -2874,12 +2873,12 @@
         <v>0</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>6</v>
@@ -2891,12 +2890,12 @@
         <v>3</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>6</v>
@@ -2908,12 +2907,12 @@
         <v>2</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>6</v>
@@ -2922,15 +2921,15 @@
         <v>20</v>
       </c>
       <c r="F69" s="4">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>6</v>
@@ -2942,12 +2941,12 @@
         <v>0</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>6</v>
@@ -2959,12 +2958,12 @@
         <v>3</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>6</v>
@@ -2973,15 +2972,15 @@
         <v>20</v>
       </c>
       <c r="F72" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>6</v>
@@ -2990,15 +2989,15 @@
         <v>50</v>
       </c>
       <c r="F73" s="4">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
@@ -3007,15 +3006,15 @@
         <v>35</v>
       </c>
       <c r="F74" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>6</v>
@@ -3024,15 +3023,15 @@
         <v>25</v>
       </c>
       <c r="F75" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>6</v>
@@ -3044,12 +3043,12 @@
         <v>1</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>6</v>
@@ -3058,15 +3057,15 @@
         <v>35</v>
       </c>
       <c r="F77" s="4">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>6</v>
@@ -3078,12 +3077,12 @@
         <v>2</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B79" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>6</v>
@@ -3092,15 +3091,15 @@
         <v>30</v>
       </c>
       <c r="F79" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B80" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>6</v>
@@ -3109,15 +3108,15 @@
         <v>35</v>
       </c>
       <c r="F80" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>6</v>
@@ -3129,12 +3128,12 @@
         <v>2</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>6</v>
@@ -3146,12 +3145,12 @@
         <v>0</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B83" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>6</v>
@@ -3160,15 +3159,15 @@
         <v>50</v>
       </c>
       <c r="F83" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B84" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>6</v>
@@ -3180,12 +3179,12 @@
         <v>0</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B85" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>6</v>
@@ -3197,12 +3196,12 @@
         <v>0</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B86" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>6</v>
@@ -3211,15 +3210,15 @@
         <v>35</v>
       </c>
       <c r="F86" s="4">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B87" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>6</v>
@@ -3231,12 +3230,12 @@
         <v>2</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B88" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>6</v>
@@ -3248,12 +3247,12 @@
         <v>0</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B89" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>6</v>
@@ -3265,12 +3264,12 @@
         <v>0</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B90" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>6</v>
@@ -3279,15 +3278,15 @@
         <v>35</v>
       </c>
       <c r="F90" s="4">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B91" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>6</v>
@@ -3299,12 +3298,12 @@
         <v>0</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B92" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>6</v>
@@ -3313,15 +3312,15 @@
         <v>35</v>
       </c>
       <c r="F92" s="4">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B93" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>6</v>
@@ -3330,15 +3329,15 @@
         <v>40</v>
       </c>
       <c r="F93" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B94" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>6</v>
@@ -3347,15 +3346,15 @@
         <v>35</v>
       </c>
       <c r="F94" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B95" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>6</v>
@@ -3367,12 +3366,12 @@
         <v>1</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B96" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>6</v>
@@ -3384,12 +3383,12 @@
         <v>0</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B97" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>6</v>
@@ -3401,12 +3400,12 @@
         <v>0</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B98" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>6</v>
@@ -3418,12 +3417,12 @@
         <v>5</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B99" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>6</v>
@@ -3435,12 +3434,12 @@
         <v>4</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B100" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>6</v>
@@ -3452,12 +3451,12 @@
         <v>0</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B101" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>6</v>
@@ -3469,12 +3468,12 @@
         <v>3</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B102" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>6</v>
@@ -3486,12 +3485,12 @@
         <v>0</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B103" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>6</v>
@@ -3503,12 +3502,12 @@
         <v>2</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B104" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>6</v>
@@ -3520,12 +3519,12 @@
         <v>0</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B105" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>6</v>
@@ -3537,12 +3536,12 @@
         <v>24</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B106" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>6</v>
@@ -3554,12 +3553,12 @@
         <v>0</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B107" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>6</v>
@@ -3571,12 +3570,12 @@
         <v>14</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B108" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>6</v>
@@ -3585,15 +3584,15 @@
         <v>10</v>
       </c>
       <c r="F108" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B109" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>6</v>
@@ -3605,12 +3604,12 @@
         <v>8</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B110" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>6</v>
@@ -3622,12 +3621,12 @@
         <v>5</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B111" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>6</v>
@@ -3636,15 +3635,15 @@
         <v>2.5</v>
       </c>
       <c r="F111" s="4">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B112" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>6</v>
@@ -3653,15 +3652,15 @@
         <v>3</v>
       </c>
       <c r="F112" s="4">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B113" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>6</v>
@@ -3673,12 +3672,12 @@
         <v>0</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B114" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>6</v>
@@ -3687,15 +3686,15 @@
         <v>20</v>
       </c>
       <c r="F114" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B115" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>6</v>
@@ -3704,15 +3703,15 @@
         <v>10</v>
       </c>
       <c r="F115" s="4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B116" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>6</v>
@@ -3721,15 +3720,15 @@
         <v>30</v>
       </c>
       <c r="F116" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B117" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>6</v>
@@ -3741,12 +3740,12 @@
         <v>0</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B118" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>6</v>
@@ -3755,15 +3754,15 @@
         <v>10</v>
       </c>
       <c r="F118" s="4">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B119" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>6</v>
@@ -3772,15 +3771,15 @@
         <v>15</v>
       </c>
       <c r="F119" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B120" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>6</v>
@@ -3792,12 +3791,12 @@
         <v>0</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B121" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>6</v>
@@ -3809,12 +3808,12 @@
         <v>0</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B122" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>6</v>
@@ -3823,15 +3822,15 @@
         <v>5</v>
       </c>
       <c r="F122" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B123" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>6</v>
@@ -3843,12 +3842,12 @@
         <v>8</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B124" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>6</v>
@@ -3860,12 +3859,12 @@
         <v>2</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B125" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>6</v>
@@ -3877,12 +3876,12 @@
         <v>0</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B126" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>6</v>
@@ -3891,15 +3890,15 @@
         <v>7</v>
       </c>
       <c r="F126" s="4">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B127" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>6</v>
@@ -3908,15 +3907,15 @@
         <v>6</v>
       </c>
       <c r="F127" s="4">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B128" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>6</v>
@@ -3925,15 +3924,15 @@
         <v>5</v>
       </c>
       <c r="F128" s="4">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B129" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>6</v>
@@ -3942,15 +3941,15 @@
         <v>10</v>
       </c>
       <c r="F129" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B130" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>6</v>
@@ -3959,15 +3958,15 @@
         <v>7</v>
       </c>
       <c r="F130" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B131" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>6</v>
@@ -3976,15 +3975,15 @@
         <v>8</v>
       </c>
       <c r="F131" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B132" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>6</v>
@@ -3993,15 +3992,15 @@
         <v>7</v>
       </c>
       <c r="F132" s="4">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B133" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>6</v>
@@ -4010,15 +4009,15 @@
         <v>7</v>
       </c>
       <c r="F133" s="4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B134" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>6</v>
@@ -4027,15 +4026,15 @@
         <v>3.5</v>
       </c>
       <c r="F134" s="4">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B135" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>6</v>
@@ -4044,15 +4043,15 @@
         <v>5</v>
       </c>
       <c r="F135" s="4">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B136" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>6</v>
@@ -4061,15 +4060,15 @@
         <v>7</v>
       </c>
       <c r="F136" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B137" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>6</v>
@@ -4081,12 +4080,12 @@
         <v>0</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B138" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>6</v>
@@ -4095,15 +4094,15 @@
         <v>7</v>
       </c>
       <c r="F138" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B139" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>6</v>
@@ -4115,12 +4114,12 @@
         <v>0</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B140" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>6</v>
@@ -4132,12 +4131,12 @@
         <v>0</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B141" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>6</v>
@@ -4146,15 +4145,15 @@
         <v>15</v>
       </c>
       <c r="F141" s="4">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B142" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>6</v>
@@ -4163,15 +4162,15 @@
         <v>2</v>
       </c>
       <c r="F142" s="4">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B143" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>6</v>
@@ -4183,12 +4182,12 @@
         <v>2</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B144" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>6</v>
@@ -4200,12 +4199,12 @@
         <v>0</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B145" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>6</v>
@@ -4217,12 +4216,12 @@
         <v>3</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B146" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>6</v>
@@ -4234,12 +4233,12 @@
         <v>0</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B147" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>6</v>
@@ -4248,15 +4247,15 @@
         <v>20</v>
       </c>
       <c r="F147">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>6</v>
@@ -4268,12 +4267,12 @@
         <v>0</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>6</v>
@@ -4285,12 +4284,12 @@
         <v>8</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B150" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>6</v>
@@ -4302,12 +4301,12 @@
         <v>0</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>6</v>
@@ -4316,15 +4315,15 @@
         <v>40</v>
       </c>
       <c r="F151">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>6</v>
@@ -4336,12 +4335,12 @@
         <v>2</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>6</v>
@@ -4353,12 +4352,12 @@
         <v>0</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>6</v>
@@ -4370,12 +4369,12 @@
         <v>1</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>6</v>
@@ -4387,12 +4386,12 @@
         <v>0</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>6</v>
@@ -4404,12 +4403,12 @@
         <v>0</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>6</v>
@@ -4421,12 +4420,12 @@
         <v>2</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B158" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>6</v>
@@ -4435,15 +4434,15 @@
         <v>30</v>
       </c>
       <c r="F158">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B159" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>6</v>
@@ -4455,12 +4454,12 @@
         <v>3</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B160" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>6</v>
@@ -4472,12 +4471,12 @@
         <v>2</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>6</v>
@@ -4486,15 +4485,15 @@
         <v>20</v>
       </c>
       <c r="F161">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>6</v>
@@ -4506,12 +4505,12 @@
         <v>1</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B163" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>6</v>
@@ -4523,12 +4522,12 @@
         <v>2</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>6</v>
@@ -4540,12 +4539,12 @@
         <v>0</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B165" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>6</v>
@@ -4557,12 +4556,12 @@
         <v>2</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B166" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>6</v>
@@ -4574,12 +4573,12 @@
         <v>11</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>6</v>
@@ -4588,15 +4587,15 @@
         <v>50</v>
       </c>
       <c r="F167">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B168" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>6</v>
@@ -4608,12 +4607,12 @@
         <v>0</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B169" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>6</v>
@@ -4622,15 +4621,15 @@
         <v>35</v>
       </c>
       <c r="F169">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G169" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B170" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>6</v>
@@ -4639,15 +4638,15 @@
         <v>10</v>
       </c>
       <c r="F170">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>6</v>
@@ -4656,15 +4655,15 @@
         <v>3.5</v>
       </c>
       <c r="F171">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B172" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>6</v>
@@ -4673,15 +4672,15 @@
         <v>3.5</v>
       </c>
       <c r="F172">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B173" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>6</v>
@@ -4690,15 +4689,15 @@
         <v>6</v>
       </c>
       <c r="F173">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B174" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>6</v>
@@ -4707,15 +4706,15 @@
         <v>6</v>
       </c>
       <c r="F174">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B175" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>6</v>
@@ -4724,15 +4723,15 @@
         <v>7</v>
       </c>
       <c r="F175">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>6</v>
@@ -4741,15 +4740,15 @@
         <v>10</v>
       </c>
       <c r="F176">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B177" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>6</v>
@@ -4758,15 +4757,15 @@
         <v>3</v>
       </c>
       <c r="F177">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B178" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>6</v>
@@ -4775,15 +4774,15 @@
         <v>5</v>
       </c>
       <c r="F178">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B179" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>6</v>
@@ -4792,15 +4791,15 @@
         <v>5</v>
       </c>
       <c r="F179">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>6</v>
@@ -4812,12 +4811,12 @@
         <v>0</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B181" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>6</v>
@@ -4829,12 +4828,12 @@
         <v>0</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>6</v>
@@ -4843,15 +4842,15 @@
         <v>16</v>
       </c>
       <c r="F182">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B183" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>6</v>
@@ -4860,15 +4859,15 @@
         <v>7</v>
       </c>
       <c r="F183">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B184" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>6</v>
@@ -4877,15 +4876,15 @@
         <v>3</v>
       </c>
       <c r="F184">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B185" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>6</v>
@@ -4894,15 +4893,15 @@
         <v>0.5</v>
       </c>
       <c r="F185">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B186" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>6</v>
@@ -4911,15 +4910,15 @@
         <v>1</v>
       </c>
       <c r="F186">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B187" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>6</v>
@@ -4928,15 +4927,15 @@
         <v>1</v>
       </c>
       <c r="F187">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G187" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B188" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>6</v>
@@ -4945,15 +4944,15 @@
         <v>0.5</v>
       </c>
       <c r="F188">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="189" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>6</v>
@@ -4965,12 +4964,12 @@
         <v>0</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="190" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B190" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>6</v>
@@ -4979,15 +4978,15 @@
         <v>1</v>
       </c>
       <c r="F190">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="191" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>6</v>
@@ -4996,15 +4995,15 @@
         <v>3</v>
       </c>
       <c r="F191">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>6</v>
@@ -5013,15 +5012,15 @@
         <v>2</v>
       </c>
       <c r="F192">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>6</v>
@@ -5030,15 +5029,15 @@
         <v>1</v>
       </c>
       <c r="F193">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="194" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>6</v>
@@ -5047,15 +5046,15 @@
         <v>0.5</v>
       </c>
       <c r="F194">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>6</v>
@@ -5064,15 +5063,15 @@
         <v>1</v>
       </c>
       <c r="F195">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="196" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B196" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>6</v>
@@ -5081,15 +5080,15 @@
         <v>2</v>
       </c>
       <c r="F196">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B197" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>6</v>
@@ -5098,15 +5097,15 @@
         <v>2</v>
       </c>
       <c r="F197">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B198" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>6</v>
@@ -5115,15 +5114,15 @@
         <v>3</v>
       </c>
       <c r="F198">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="199" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B199" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>6</v>
@@ -5132,15 +5131,15 @@
         <v>4</v>
       </c>
       <c r="F199">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G199" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="200" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B200" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>6</v>
@@ -5149,15 +5148,15 @@
         <v>3</v>
       </c>
       <c r="F200">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="201" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B201" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>6</v>
@@ -5166,15 +5165,15 @@
         <v>3</v>
       </c>
       <c r="F201">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="202" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B202" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>6</v>
@@ -5183,15 +5182,15 @@
         <v>2</v>
       </c>
       <c r="F202">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="203" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B203" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>6</v>
@@ -5200,15 +5199,15 @@
         <v>2</v>
       </c>
       <c r="F203">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G203" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="204" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B204" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>6</v>
@@ -5217,15 +5216,15 @@
         <v>3</v>
       </c>
       <c r="F204">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="205" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B205" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>6</v>
@@ -5234,32 +5233,32 @@
         <v>1</v>
       </c>
       <c r="F205">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G205" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="206" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B206" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E206" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F206">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="207" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B207" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>6</v>
@@ -5268,15 +5267,15 @@
         <v>2.5</v>
       </c>
       <c r="F207">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G207" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="208" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>6</v>
@@ -5285,15 +5284,15 @@
         <v>3.5</v>
       </c>
       <c r="F208">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="209" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B209" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>6</v>
@@ -5302,15 +5301,15 @@
         <v>3.5</v>
       </c>
       <c r="F209">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B210" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>6</v>
@@ -5319,15 +5318,15 @@
         <v>2.5</v>
       </c>
       <c r="F210">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="211" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B211" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>6</v>
@@ -5336,15 +5335,15 @@
         <v>2.5</v>
       </c>
       <c r="F211">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="G211" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B212" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D212" s="2" t="s">
         <v>6</v>
@@ -5353,15 +5352,15 @@
         <v>7</v>
       </c>
       <c r="F212">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="213" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B213" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>6</v>
@@ -5373,11 +5372,11 @@
         <v>0</v>
       </c>
       <c r="G213" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G213" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G213"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>